<commit_message>
report section is completed
</commit_message>
<xml_diff>
--- a/public/report_templates/anesthesias_report.xlsx
+++ b/public/report_templates/anesthesias_report.xlsx
@@ -19,30 +19,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>شماره</t>
   </si>
   <si>
-    <t>جنس</t>
+    <t>راپور انستیزی ها</t>
   </si>
   <si>
-    <t>تعداد</t>
+    <t>اسم مریض</t>
   </si>
   <si>
-    <t>راپور جمع و قید اجناس</t>
+    <t>حالت</t>
   </si>
   <si>
-    <t>اسم</t>
+    <t>نام داکتر</t>
   </si>
   <si>
-    <t>اسم پدر</t>
+    <t>نوعیت انستیزی</t>
   </si>
   <si>
-    <t>شماره کارت</t>
+    <t>شفاخانه</t>
   </si>
   <si>
-    <t>توضیحات</t>
+    <t>تاریخ</t>
+  </si>
+  <si>
+    <t>ساعت</t>
   </si>
 </sst>
 </file>
@@ -86,7 +89,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -109,17 +112,56 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -402,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G112"/>
+  <dimension ref="A1:H140"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -419,41 +461,45 @@
     <col min="7" max="7" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+    </row>
+    <row r="2" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-    </row>
-    <row r="2" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="E2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="F2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -461,8 +507,9 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -470,8 +517,9 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -479,8 +527,9 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -488,8 +537,9 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -497,8 +547,9 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -506,8 +557,9 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -515,8 +567,9 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -524,8 +577,9 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -533,8 +587,9 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -542,8 +597,9 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -551,8 +607,9 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -560,8 +617,9 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -569,8 +627,9 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H15" s="1"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -578,8 +637,9 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H16" s="1"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -587,8 +647,9 @@
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H17" s="1"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -596,8 +657,9 @@
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H18" s="1"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -605,8 +667,9 @@
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H19" s="1"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -614,8 +677,9 @@
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H20" s="1"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -623,8 +687,9 @@
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H21" s="1"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -632,8 +697,9 @@
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H22" s="1"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -641,8 +707,9 @@
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H23" s="1"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -650,8 +717,9 @@
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H24" s="1"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -659,8 +727,9 @@
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H25" s="1"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -668,8 +737,9 @@
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H26" s="1"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -677,8 +747,9 @@
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H27" s="1"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -686,8 +757,9 @@
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H28" s="1"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -695,8 +767,9 @@
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H29" s="1"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -704,8 +777,9 @@
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H30" s="1"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -713,8 +787,9 @@
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H31" s="1"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -722,8 +797,9 @@
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H32" s="1"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -731,8 +807,9 @@
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H33" s="1"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -740,8 +817,9 @@
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H34" s="1"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -749,8 +827,9 @@
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H35" s="1"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -758,8 +837,9 @@
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H36" s="1"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -767,8 +847,9 @@
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H37" s="1"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -776,8 +857,9 @@
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H38" s="1"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -785,8 +867,9 @@
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H39" s="1"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -794,8 +877,9 @@
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H40" s="1"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -803,8 +887,9 @@
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H41" s="1"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -812,8 +897,9 @@
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H42" s="1"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -821,8 +907,9 @@
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H43" s="1"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -830,8 +917,9 @@
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H44" s="1"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -839,8 +927,9 @@
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H45" s="1"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -848,8 +937,9 @@
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H46" s="1"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -857,8 +947,9 @@
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H47" s="1"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -866,8 +957,9 @@
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H48" s="1"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -875,8 +967,9 @@
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H49" s="1"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -884,8 +977,9 @@
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H50" s="1"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -893,8 +987,9 @@
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H51" s="1"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -902,8 +997,9 @@
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H52" s="1"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -911,8 +1007,9 @@
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H53" s="1"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -920,8 +1017,9 @@
       <c r="E54" s="1"/>
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H54" s="1"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -929,8 +1027,9 @@
       <c r="E55" s="1"/>
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H55" s="1"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -938,8 +1037,9 @@
       <c r="E56" s="1"/>
       <c r="F56" s="1"/>
       <c r="G56" s="1"/>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H56" s="1"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -947,8 +1047,9 @@
       <c r="E57" s="1"/>
       <c r="F57" s="1"/>
       <c r="G57" s="1"/>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H57" s="1"/>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -956,8 +1057,9 @@
       <c r="E58" s="1"/>
       <c r="F58" s="1"/>
       <c r="G58" s="1"/>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H58" s="1"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -965,8 +1067,9 @@
       <c r="E59" s="1"/>
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H59" s="1"/>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -974,8 +1077,9 @@
       <c r="E60" s="1"/>
       <c r="F60" s="1"/>
       <c r="G60" s="1"/>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H60" s="1"/>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -983,8 +1087,9 @@
       <c r="E61" s="1"/>
       <c r="F61" s="1"/>
       <c r="G61" s="1"/>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H61" s="1"/>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -992,8 +1097,9 @@
       <c r="E62" s="1"/>
       <c r="F62" s="1"/>
       <c r="G62" s="1"/>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H62" s="1"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -1001,8 +1107,9 @@
       <c r="E63" s="1"/>
       <c r="F63" s="1"/>
       <c r="G63" s="1"/>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H63" s="1"/>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -1010,8 +1117,9 @@
       <c r="E64" s="1"/>
       <c r="F64" s="1"/>
       <c r="G64" s="1"/>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H64" s="1"/>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -1019,8 +1127,9 @@
       <c r="E65" s="1"/>
       <c r="F65" s="1"/>
       <c r="G65" s="1"/>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H65" s="1"/>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -1028,8 +1137,9 @@
       <c r="E66" s="1"/>
       <c r="F66" s="1"/>
       <c r="G66" s="1"/>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H66" s="1"/>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -1037,8 +1147,9 @@
       <c r="E67" s="1"/>
       <c r="F67" s="1"/>
       <c r="G67" s="1"/>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H67" s="1"/>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -1046,8 +1157,9 @@
       <c r="E68" s="1"/>
       <c r="F68" s="1"/>
       <c r="G68" s="1"/>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H68" s="1"/>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -1055,8 +1167,9 @@
       <c r="E69" s="1"/>
       <c r="F69" s="1"/>
       <c r="G69" s="1"/>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H69" s="1"/>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -1064,8 +1177,9 @@
       <c r="E70" s="1"/>
       <c r="F70" s="1"/>
       <c r="G70" s="1"/>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H70" s="1"/>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -1073,8 +1187,9 @@
       <c r="E71" s="1"/>
       <c r="F71" s="1"/>
       <c r="G71" s="1"/>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H71" s="1"/>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -1082,8 +1197,9 @@
       <c r="E72" s="1"/>
       <c r="F72" s="1"/>
       <c r="G72" s="1"/>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H72" s="1"/>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -1091,8 +1207,9 @@
       <c r="E73" s="1"/>
       <c r="F73" s="1"/>
       <c r="G73" s="1"/>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H73" s="1"/>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -1100,8 +1217,9 @@
       <c r="E74" s="1"/>
       <c r="F74" s="1"/>
       <c r="G74" s="1"/>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H74" s="1"/>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -1109,8 +1227,9 @@
       <c r="E75" s="1"/>
       <c r="F75" s="1"/>
       <c r="G75" s="1"/>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H75" s="1"/>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -1118,8 +1237,9 @@
       <c r="E76" s="1"/>
       <c r="F76" s="1"/>
       <c r="G76" s="1"/>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H76" s="1"/>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -1127,8 +1247,9 @@
       <c r="E77" s="1"/>
       <c r="F77" s="1"/>
       <c r="G77" s="1"/>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H77" s="1"/>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -1136,8 +1257,9 @@
       <c r="E78" s="1"/>
       <c r="F78" s="1"/>
       <c r="G78" s="1"/>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H78" s="1"/>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -1145,8 +1267,9 @@
       <c r="E79" s="1"/>
       <c r="F79" s="1"/>
       <c r="G79" s="1"/>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H79" s="1"/>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -1154,8 +1277,9 @@
       <c r="E80" s="1"/>
       <c r="F80" s="1"/>
       <c r="G80" s="1"/>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H80" s="1"/>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -1163,8 +1287,9 @@
       <c r="E81" s="1"/>
       <c r="F81" s="1"/>
       <c r="G81" s="1"/>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H81" s="1"/>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -1172,8 +1297,9 @@
       <c r="E82" s="1"/>
       <c r="F82" s="1"/>
       <c r="G82" s="1"/>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H82" s="1"/>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -1181,8 +1307,9 @@
       <c r="E83" s="1"/>
       <c r="F83" s="1"/>
       <c r="G83" s="1"/>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H83" s="1"/>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
@@ -1190,8 +1317,9 @@
       <c r="E84" s="1"/>
       <c r="F84" s="1"/>
       <c r="G84" s="1"/>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H84" s="1"/>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -1199,8 +1327,9 @@
       <c r="E85" s="1"/>
       <c r="F85" s="1"/>
       <c r="G85" s="1"/>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H85" s="1"/>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
@@ -1208,8 +1337,9 @@
       <c r="E86" s="1"/>
       <c r="F86" s="1"/>
       <c r="G86" s="1"/>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H86" s="1"/>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
@@ -1217,8 +1347,9 @@
       <c r="E87" s="1"/>
       <c r="F87" s="1"/>
       <c r="G87" s="1"/>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H87" s="1"/>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -1226,8 +1357,9 @@
       <c r="E88" s="1"/>
       <c r="F88" s="1"/>
       <c r="G88" s="1"/>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H88" s="1"/>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
@@ -1235,8 +1367,9 @@
       <c r="E89" s="1"/>
       <c r="F89" s="1"/>
       <c r="G89" s="1"/>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H89" s="1"/>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
@@ -1244,8 +1377,9 @@
       <c r="E90" s="1"/>
       <c r="F90" s="1"/>
       <c r="G90" s="1"/>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H90" s="1"/>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
@@ -1253,8 +1387,9 @@
       <c r="E91" s="1"/>
       <c r="F91" s="1"/>
       <c r="G91" s="1"/>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H91" s="1"/>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
@@ -1262,8 +1397,9 @@
       <c r="E92" s="1"/>
       <c r="F92" s="1"/>
       <c r="G92" s="1"/>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H92" s="1"/>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
@@ -1271,8 +1407,9 @@
       <c r="E93" s="1"/>
       <c r="F93" s="1"/>
       <c r="G93" s="1"/>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H93" s="1"/>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
@@ -1280,8 +1417,9 @@
       <c r="E94" s="1"/>
       <c r="F94" s="1"/>
       <c r="G94" s="1"/>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H94" s="1"/>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
@@ -1289,8 +1427,9 @@
       <c r="E95" s="1"/>
       <c r="F95" s="1"/>
       <c r="G95" s="1"/>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H95" s="1"/>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
@@ -1298,8 +1437,9 @@
       <c r="E96" s="1"/>
       <c r="F96" s="1"/>
       <c r="G96" s="1"/>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H96" s="1"/>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
@@ -1307,8 +1447,9 @@
       <c r="E97" s="1"/>
       <c r="F97" s="1"/>
       <c r="G97" s="1"/>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H97" s="1"/>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
@@ -1316,8 +1457,9 @@
       <c r="E98" s="1"/>
       <c r="F98" s="1"/>
       <c r="G98" s="1"/>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H98" s="1"/>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
@@ -1325,8 +1467,9 @@
       <c r="E99" s="1"/>
       <c r="F99" s="1"/>
       <c r="G99" s="1"/>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H99" s="1"/>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
@@ -1334,8 +1477,9 @@
       <c r="E100" s="1"/>
       <c r="F100" s="1"/>
       <c r="G100" s="1"/>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H100" s="1"/>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="1"/>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
@@ -1343,8 +1487,9 @@
       <c r="E101" s="1"/>
       <c r="F101" s="1"/>
       <c r="G101" s="1"/>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H101" s="1"/>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
@@ -1352,8 +1497,9 @@
       <c r="E102" s="1"/>
       <c r="F102" s="1"/>
       <c r="G102" s="1"/>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H102" s="1"/>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="1"/>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
@@ -1361,8 +1507,9 @@
       <c r="E103" s="1"/>
       <c r="F103" s="1"/>
       <c r="G103" s="1"/>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H103" s="1"/>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" s="1"/>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
@@ -1370,8 +1517,9 @@
       <c r="E104" s="1"/>
       <c r="F104" s="1"/>
       <c r="G104" s="1"/>
-    </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H104" s="1"/>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="1"/>
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
@@ -1379,8 +1527,9 @@
       <c r="E105" s="1"/>
       <c r="F105" s="1"/>
       <c r="G105" s="1"/>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H105" s="1"/>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" s="1"/>
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
@@ -1388,8 +1537,9 @@
       <c r="E106" s="1"/>
       <c r="F106" s="1"/>
       <c r="G106" s="1"/>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H106" s="1"/>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" s="1"/>
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
@@ -1397,8 +1547,9 @@
       <c r="E107" s="1"/>
       <c r="F107" s="1"/>
       <c r="G107" s="1"/>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H107" s="1"/>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" s="1"/>
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
@@ -1406,8 +1557,9 @@
       <c r="E108" s="1"/>
       <c r="F108" s="1"/>
       <c r="G108" s="1"/>
-    </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H108" s="1"/>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" s="1"/>
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
@@ -1415,8 +1567,9 @@
       <c r="E109" s="1"/>
       <c r="F109" s="1"/>
       <c r="G109" s="1"/>
-    </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H109" s="1"/>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" s="1"/>
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
@@ -1424,8 +1577,9 @@
       <c r="E110" s="1"/>
       <c r="F110" s="1"/>
       <c r="G110" s="1"/>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H110" s="1"/>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" s="1"/>
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
@@ -1433,8 +1587,9 @@
       <c r="E111" s="1"/>
       <c r="F111" s="1"/>
       <c r="G111" s="1"/>
-    </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H111" s="1"/>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" s="1"/>
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
@@ -1442,10 +1597,291 @@
       <c r="E112" s="1"/>
       <c r="F112" s="1"/>
       <c r="G112" s="1"/>
+      <c r="H112" s="1"/>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A113" s="1"/>
+      <c r="B113" s="1"/>
+      <c r="C113" s="1"/>
+      <c r="D113" s="1"/>
+      <c r="E113" s="1"/>
+      <c r="F113" s="1"/>
+      <c r="G113" s="1"/>
+      <c r="H113" s="1"/>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A114" s="1"/>
+      <c r="B114" s="1"/>
+      <c r="C114" s="1"/>
+      <c r="D114" s="1"/>
+      <c r="E114" s="1"/>
+      <c r="F114" s="1"/>
+      <c r="G114" s="1"/>
+      <c r="H114" s="1"/>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A115" s="1"/>
+      <c r="B115" s="1"/>
+      <c r="C115" s="1"/>
+      <c r="D115" s="1"/>
+      <c r="E115" s="1"/>
+      <c r="F115" s="1"/>
+      <c r="G115" s="1"/>
+      <c r="H115" s="1"/>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A116" s="1"/>
+      <c r="B116" s="1"/>
+      <c r="C116" s="1"/>
+      <c r="D116" s="1"/>
+      <c r="E116" s="1"/>
+      <c r="F116" s="1"/>
+      <c r="G116" s="1"/>
+      <c r="H116" s="1"/>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A117" s="1"/>
+      <c r="B117" s="1"/>
+      <c r="C117" s="1"/>
+      <c r="D117" s="1"/>
+      <c r="E117" s="1"/>
+      <c r="F117" s="1"/>
+      <c r="G117" s="1"/>
+      <c r="H117" s="1"/>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A118" s="1"/>
+      <c r="B118" s="1"/>
+      <c r="C118" s="1"/>
+      <c r="D118" s="1"/>
+      <c r="E118" s="1"/>
+      <c r="F118" s="1"/>
+      <c r="G118" s="1"/>
+      <c r="H118" s="1"/>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A119" s="1"/>
+      <c r="B119" s="1"/>
+      <c r="C119" s="1"/>
+      <c r="D119" s="1"/>
+      <c r="E119" s="1"/>
+      <c r="F119" s="1"/>
+      <c r="G119" s="1"/>
+      <c r="H119" s="1"/>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A120" s="1"/>
+      <c r="B120" s="1"/>
+      <c r="C120" s="1"/>
+      <c r="D120" s="1"/>
+      <c r="E120" s="1"/>
+      <c r="F120" s="1"/>
+      <c r="G120" s="1"/>
+      <c r="H120" s="1"/>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A121" s="1"/>
+      <c r="B121" s="1"/>
+      <c r="C121" s="1"/>
+      <c r="D121" s="1"/>
+      <c r="E121" s="1"/>
+      <c r="F121" s="1"/>
+      <c r="G121" s="1"/>
+      <c r="H121" s="1"/>
+    </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A122" s="1"/>
+      <c r="B122" s="1"/>
+      <c r="C122" s="1"/>
+      <c r="D122" s="1"/>
+      <c r="E122" s="1"/>
+      <c r="F122" s="1"/>
+      <c r="G122" s="1"/>
+      <c r="H122" s="1"/>
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A123" s="1"/>
+      <c r="B123" s="1"/>
+      <c r="C123" s="1"/>
+      <c r="D123" s="1"/>
+      <c r="E123" s="1"/>
+      <c r="F123" s="1"/>
+      <c r="G123" s="1"/>
+      <c r="H123" s="1"/>
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A124" s="1"/>
+      <c r="B124" s="1"/>
+      <c r="C124" s="1"/>
+      <c r="D124" s="1"/>
+      <c r="E124" s="1"/>
+      <c r="F124" s="1"/>
+      <c r="G124" s="1"/>
+      <c r="H124" s="1"/>
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A125" s="1"/>
+      <c r="B125" s="1"/>
+      <c r="C125" s="1"/>
+      <c r="D125" s="1"/>
+      <c r="E125" s="1"/>
+      <c r="F125" s="1"/>
+      <c r="G125" s="1"/>
+      <c r="H125" s="1"/>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A126" s="1"/>
+      <c r="B126" s="1"/>
+      <c r="C126" s="1"/>
+      <c r="D126" s="1"/>
+      <c r="E126" s="1"/>
+      <c r="F126" s="1"/>
+      <c r="G126" s="1"/>
+      <c r="H126" s="1"/>
+    </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A127" s="1"/>
+      <c r="B127" s="1"/>
+      <c r="C127" s="1"/>
+      <c r="D127" s="1"/>
+      <c r="E127" s="1"/>
+      <c r="F127" s="1"/>
+      <c r="G127" s="1"/>
+      <c r="H127" s="1"/>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A128" s="1"/>
+      <c r="B128" s="1"/>
+      <c r="C128" s="1"/>
+      <c r="D128" s="1"/>
+      <c r="E128" s="1"/>
+      <c r="F128" s="1"/>
+      <c r="G128" s="1"/>
+      <c r="H128" s="1"/>
+    </row>
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A129" s="1"/>
+      <c r="B129" s="1"/>
+      <c r="C129" s="1"/>
+      <c r="D129" s="1"/>
+      <c r="E129" s="1"/>
+      <c r="F129" s="1"/>
+      <c r="G129" s="1"/>
+      <c r="H129" s="1"/>
+    </row>
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A130" s="1"/>
+      <c r="B130" s="1"/>
+      <c r="C130" s="1"/>
+      <c r="D130" s="1"/>
+      <c r="E130" s="1"/>
+      <c r="F130" s="1"/>
+      <c r="G130" s="1"/>
+      <c r="H130" s="1"/>
+    </row>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A131" s="1"/>
+      <c r="B131" s="1"/>
+      <c r="C131" s="1"/>
+      <c r="D131" s="1"/>
+      <c r="E131" s="1"/>
+      <c r="F131" s="1"/>
+      <c r="G131" s="1"/>
+      <c r="H131" s="1"/>
+    </row>
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A132" s="1"/>
+      <c r="B132" s="1"/>
+      <c r="C132" s="1"/>
+      <c r="D132" s="1"/>
+      <c r="E132" s="1"/>
+      <c r="F132" s="1"/>
+      <c r="G132" s="1"/>
+      <c r="H132" s="1"/>
+    </row>
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A133" s="1"/>
+      <c r="B133" s="1"/>
+      <c r="C133" s="1"/>
+      <c r="D133" s="1"/>
+      <c r="E133" s="1"/>
+      <c r="F133" s="1"/>
+      <c r="G133" s="1"/>
+      <c r="H133" s="1"/>
+    </row>
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A134" s="1"/>
+      <c r="B134" s="1"/>
+      <c r="C134" s="1"/>
+      <c r="D134" s="1"/>
+      <c r="E134" s="1"/>
+      <c r="F134" s="1"/>
+      <c r="G134" s="1"/>
+      <c r="H134" s="1"/>
+    </row>
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A135" s="1"/>
+      <c r="B135" s="1"/>
+      <c r="C135" s="1"/>
+      <c r="D135" s="1"/>
+      <c r="E135" s="1"/>
+      <c r="F135" s="1"/>
+      <c r="G135" s="1"/>
+      <c r="H135" s="1"/>
+    </row>
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A136" s="1"/>
+      <c r="B136" s="1"/>
+      <c r="C136" s="1"/>
+      <c r="D136" s="1"/>
+      <c r="E136" s="1"/>
+      <c r="F136" s="1"/>
+      <c r="G136" s="1"/>
+      <c r="H136" s="1"/>
+    </row>
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A137" s="1"/>
+      <c r="B137" s="1"/>
+      <c r="C137" s="1"/>
+      <c r="D137" s="1"/>
+      <c r="E137" s="1"/>
+      <c r="F137" s="1"/>
+      <c r="G137" s="1"/>
+      <c r="H137" s="1"/>
+    </row>
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A138" s="1"/>
+      <c r="B138" s="1"/>
+      <c r="C138" s="1"/>
+      <c r="D138" s="1"/>
+      <c r="E138" s="1"/>
+      <c r="F138" s="1"/>
+      <c r="G138" s="1"/>
+      <c r="H138" s="1"/>
+    </row>
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A139" s="1"/>
+      <c r="B139" s="1"/>
+      <c r="C139" s="1"/>
+      <c r="D139" s="1"/>
+      <c r="E139" s="1"/>
+      <c r="F139" s="1"/>
+      <c r="G139" s="1"/>
+      <c r="H139" s="1"/>
+    </row>
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A140" s="1"/>
+      <c r="B140" s="1"/>
+      <c r="C140" s="1"/>
+      <c r="D140" s="1"/>
+      <c r="E140" s="1"/>
+      <c r="F140" s="1"/>
+      <c r="G140" s="1"/>
+      <c r="H140" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>